<commit_message>
Added Excel Data Map & Hover scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/config/test.xlsx
+++ b/src/test/resources/config/test.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22206"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{090C02FB-CDC8-4998-BA9E-276C197205B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet10" sheetId="1" r:id="rId1"/>
+    <sheet name="Item Filter" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -35,13 +45,61 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>TC ID</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>tc_01</t>
+  </si>
+  <si>
+    <t>Summer Dresses</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>In stock</t>
+  </si>
+  <si>
+    <t>tc_02</t>
+  </si>
+  <si>
+    <t>Casual Dresses</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>tc_03</t>
+  </si>
+  <si>
+    <t>Evening Dresses</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +223,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -200,6 +275,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,16 +467,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -410,6 +502,93 @@
       </c>
       <c r="D2">
         <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEF98D9-DD45-40D2-8DFD-A83FFEF6956F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel reader step
</commit_message>
<xml_diff>
--- a/src/test/resources/config/test.xlsx
+++ b/src/test/resources/config/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22206"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{090C02FB-CDC8-4998-BA9E-276C197205B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A950CF78-C826-4E3E-B604-CB3E588D5CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>firstname</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>Yellow</t>
   </si>
   <si>
     <t>In stock</t>
@@ -514,7 +511,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,45 +547,36 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>